<commit_message>
UI Updated for Multi Query and getting on-demand price from pricing api is updated to getting price from db table
</commit_message>
<xml_diff>
--- a/assets/Sample_Input_template.xlsx
+++ b/assets/Sample_Input_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FNS\Desktop\AWS-PC - Copy\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DE0B14-9384-488F-8C39-1A90E86D6776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F01C3A-F6EB-4D5C-AE61-CFBC7C441A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{4E35BF92-FBCE-427E-9639-716A630E945F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>DNS Name</t>
   </si>
@@ -506,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3477A29-ABDE-45B5-B81D-4FAAD9626EF6}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,31 +651,6 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>